<commit_message>
Minor edits to the Figures. Reviewed non-DOI articles now.
</commit_message>
<xml_diff>
--- a/R/DATA-RAW/papers2.xlsx
+++ b/R/DATA-RAW/papers2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbrky\Desktop\School\Aging and Heat\cc-aging-review\R\DATA-RAW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fsu-my.sharepoint.com/personal/meh03c_fsu_edu/Documents/MANUSCRIPTS/WORKING/cc-aging-review/R/DATA-RAW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE70B62C-02DA-415C-B7A9-E1D7251D3D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{DE70B62C-02DA-415C-B7A9-E1D7251D3D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A07B07B-9CB6-403C-A8A1-4F7A52DD3AB4}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="4313" windowWidth="20715" windowHeight="13275" tabRatio="184" xr2:uid="{0474FF3C-F5F4-4032-A5CB-9951DE8E4272}"/>
+    <workbookView xWindow="30615" yWindow="690" windowWidth="25635" windowHeight="14295" tabRatio="184" xr2:uid="{0474FF3C-F5F4-4032-A5CB-9951DE8E4272}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19857" uniqueCount="3809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20033" uniqueCount="3839">
   <si>
     <t>AU</t>
   </si>
@@ -11801,6 +11801,96 @@
   </si>
   <si>
     <t>leisure activities</t>
+  </si>
+  <si>
+    <t>Bontemps, Jean-Daniel; Herve, Jean-Christophe; Dhote, Jean-Francois</t>
+  </si>
+  <si>
+    <t>Long-Term Changes in Forest Productivity: A Consistent Assessment in Even-Aged Stands</t>
+  </si>
+  <si>
+    <t>WOS:000272691000008</t>
+  </si>
+  <si>
+    <t>North, M; Hurteau, M; Fiegener, R; Barbour, M</t>
+  </si>
+  <si>
+    <t>Influence of fire and El Nino on tree recruitment varies by species in Sierran mixed conifer</t>
+  </si>
+  <si>
+    <t>WOS:000229764500002</t>
+  </si>
+  <si>
+    <t>Gower, ST; Krankina, O; Olson, RJ; Apps, M; Linder, S; Wang, C</t>
+  </si>
+  <si>
+    <t>Net primary production and carbon allocation patterns of boreal forest ecosystems</t>
+  </si>
+  <si>
+    <t>WOS:000171417700012</t>
+  </si>
+  <si>
+    <t>Greenhill, J. A.; Walker, J.; Playford, D.</t>
+  </si>
+  <si>
+    <t>Outcomes of Australian rural clinical schools: a decade of success building the rural medical workforce through the education and training continuum</t>
+  </si>
+  <si>
+    <t>WOS:000365601800005</t>
+  </si>
+  <si>
+    <t>Murray, Dennis L.; Cox, Eric W.; Ballard, Warren B.; Whitlaw, Heather A.; Lenarz, Mark S.; Custer, Thomas W.; Barnett, Terri; Fuller, Todd K.</t>
+  </si>
+  <si>
+    <t>Pathogens, nutritional deficiency, and climate influences on a declining moose population</t>
+  </si>
+  <si>
+    <t>WOS:000244136000001</t>
+  </si>
+  <si>
+    <t>Hickman, Caroline; Marks, Elizabeth; Pihkala, Panu; Clayton, Susan; Lewandowski, R. Eric; Mayall, Elouise E.; Wray, Britt; Mellor, Catriona; van Susteren, Lise</t>
+  </si>
+  <si>
+    <t>Climate anxiety in children and young people and their beliefs about government responses to climate change: a global survey</t>
+  </si>
+  <si>
+    <t>WOS:000730800800010</t>
+  </si>
+  <si>
+    <t>Jay, Ollie; Capon, Anthony; Berry, Peter; Broderick, Carolyn; de Dear, Richard; Havenith, George; Honda, Yasushi; Kovats, R. Sari; Ma, Wei; Malik, Arunima; Morris, Nathan B.; Nybo, Lars; Seneviratne, Sonia I.; Vanos, Jennifer; Ebi, Kristie L.</t>
+  </si>
+  <si>
+    <t>Reducing the health effects of hot weather and heat extremes: from personal cooling strategies to green cities</t>
+  </si>
+  <si>
+    <t>WOS:000687280700027</t>
+  </si>
+  <si>
+    <t>Hellden, Daniel; Andersson, Camilla; Nilsson, Maria; Ebi, Kristie L.; Friberg, Peter; Alfven, Tobias</t>
+  </si>
+  <si>
+    <t>Climate change and child health: a scoping review and an expanded conceptual framework</t>
+  </si>
+  <si>
+    <t>WOS:000629882600010</t>
+  </si>
+  <si>
+    <t>Deals with Forests</t>
+  </si>
+  <si>
+    <t>About mooses</t>
+  </si>
+  <si>
+    <t>About children</t>
+  </si>
+  <si>
+    <t>About rural clinical schools</t>
+  </si>
+  <si>
+    <t>Primarily about exreme heat and air conditioning. It’s a review article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We summarise the benefits (eg, effectiveness) and limitations of each identified cooling strategy, and recommend optimal interventions for settings such as aged care homes, slums, workplaces, mass gatherings, refugee camps, and playing sport. </t>
   </si>
 </sst>
 </file>
@@ -12207,10 +12297,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE7EB28-56C6-4661-A107-FC24E54E6505}">
-  <dimension ref="A1:AC600"/>
+  <dimension ref="A1:AC608"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R246" sqref="R246"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA607" sqref="AA607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67044,6 +67135,750 @@
         <v>41</v>
       </c>
     </row>
+    <row r="601" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B601" t="s">
+        <v>3810</v>
+      </c>
+      <c r="C601" t="s">
+        <v>33</v>
+      </c>
+      <c r="D601">
+        <v>2009</v>
+      </c>
+      <c r="E601">
+        <v>72</v>
+      </c>
+      <c r="F601" t="s">
+        <v>3811</v>
+      </c>
+      <c r="G601" t="s">
+        <v>126</v>
+      </c>
+      <c r="H601" t="s">
+        <v>36</v>
+      </c>
+      <c r="I601" t="s">
+        <v>33</v>
+      </c>
+      <c r="J601" t="str">
+        <f>B601</f>
+        <v>Long-Term Changes in Forest Productivity: A Consistent Assessment in Even-Aged Stands</v>
+      </c>
+      <c r="K601" t="str">
+        <f>A601</f>
+        <v>Bontemps, Jean-Daniel; Herve, Jean-Christophe; Dhote, Jean-Francois</v>
+      </c>
+      <c r="L601">
+        <f>E601</f>
+        <v>72</v>
+      </c>
+      <c r="M601">
+        <f>L601/(2023-D601)</f>
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="N601" t="s">
+        <v>34</v>
+      </c>
+      <c r="O601" t="s">
+        <v>3833</v>
+      </c>
+      <c r="P601" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q601" t="s">
+        <v>33</v>
+      </c>
+      <c r="R601" t="s">
+        <v>33</v>
+      </c>
+      <c r="S601" t="s">
+        <v>33</v>
+      </c>
+      <c r="T601" t="s">
+        <v>33</v>
+      </c>
+      <c r="U601" t="s">
+        <v>33</v>
+      </c>
+      <c r="V601" t="s">
+        <v>33</v>
+      </c>
+      <c r="W601" t="s">
+        <v>33</v>
+      </c>
+      <c r="X601" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y601" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z601" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA601" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB601">
+        <v>0</v>
+      </c>
+      <c r="AC601" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="602" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B602" t="s">
+        <v>3813</v>
+      </c>
+      <c r="C602" t="s">
+        <v>33</v>
+      </c>
+      <c r="D602">
+        <v>2005</v>
+      </c>
+      <c r="E602">
+        <v>80</v>
+      </c>
+      <c r="F602" t="s">
+        <v>3814</v>
+      </c>
+      <c r="G602" t="s">
+        <v>126</v>
+      </c>
+      <c r="H602" t="s">
+        <v>36</v>
+      </c>
+      <c r="I602" t="s">
+        <v>33</v>
+      </c>
+      <c r="J602" t="str">
+        <f t="shared" ref="J602:J608" si="0">B602</f>
+        <v>Influence of fire and El Nino on tree recruitment varies by species in Sierran mixed conifer</v>
+      </c>
+      <c r="K602" t="str">
+        <f t="shared" ref="K602:K608" si="1">A602</f>
+        <v>North, M; Hurteau, M; Fiegener, R; Barbour, M</v>
+      </c>
+      <c r="L602">
+        <f t="shared" ref="L602:L608" si="2">E602</f>
+        <v>80</v>
+      </c>
+      <c r="M602">
+        <f t="shared" ref="M602:M608" si="3">L602/(2023-D602)</f>
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="N602" t="s">
+        <v>34</v>
+      </c>
+      <c r="O602" t="s">
+        <v>3833</v>
+      </c>
+      <c r="P602" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q602" t="s">
+        <v>33</v>
+      </c>
+      <c r="R602" t="s">
+        <v>33</v>
+      </c>
+      <c r="S602" t="s">
+        <v>33</v>
+      </c>
+      <c r="T602" t="s">
+        <v>33</v>
+      </c>
+      <c r="U602" t="s">
+        <v>33</v>
+      </c>
+      <c r="V602" t="s">
+        <v>33</v>
+      </c>
+      <c r="W602" t="s">
+        <v>33</v>
+      </c>
+      <c r="X602" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y602" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z602" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA602" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB602">
+        <v>0</v>
+      </c>
+      <c r="AC602" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="603" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>3815</v>
+      </c>
+      <c r="B603" t="s">
+        <v>3816</v>
+      </c>
+      <c r="C603" t="s">
+        <v>33</v>
+      </c>
+      <c r="D603">
+        <v>2001</v>
+      </c>
+      <c r="E603">
+        <v>326</v>
+      </c>
+      <c r="F603" t="s">
+        <v>3817</v>
+      </c>
+      <c r="G603" t="s">
+        <v>126</v>
+      </c>
+      <c r="H603" t="s">
+        <v>36</v>
+      </c>
+      <c r="I603" t="s">
+        <v>33</v>
+      </c>
+      <c r="J603" t="str">
+        <f t="shared" si="0"/>
+        <v>Net primary production and carbon allocation patterns of boreal forest ecosystems</v>
+      </c>
+      <c r="K603" t="str">
+        <f t="shared" si="1"/>
+        <v>Gower, ST; Krankina, O; Olson, RJ; Apps, M; Linder, S; Wang, C</v>
+      </c>
+      <c r="L603">
+        <f t="shared" si="2"/>
+        <v>326</v>
+      </c>
+      <c r="M603">
+        <f t="shared" si="3"/>
+        <v>14.818181818181818</v>
+      </c>
+      <c r="N603" t="s">
+        <v>34</v>
+      </c>
+      <c r="O603" t="s">
+        <v>3833</v>
+      </c>
+      <c r="P603" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q603" t="s">
+        <v>33</v>
+      </c>
+      <c r="R603" t="s">
+        <v>33</v>
+      </c>
+      <c r="S603" t="s">
+        <v>33</v>
+      </c>
+      <c r="T603" t="s">
+        <v>33</v>
+      </c>
+      <c r="U603" t="s">
+        <v>33</v>
+      </c>
+      <c r="V603" t="s">
+        <v>33</v>
+      </c>
+      <c r="W603" t="s">
+        <v>33</v>
+      </c>
+      <c r="X603" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y603" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z603" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA603" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB603">
+        <v>0</v>
+      </c>
+      <c r="AC603" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="604" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B604" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C604" t="s">
+        <v>33</v>
+      </c>
+      <c r="D604">
+        <v>2015</v>
+      </c>
+      <c r="E604">
+        <v>53</v>
+      </c>
+      <c r="F604" t="s">
+        <v>3820</v>
+      </c>
+      <c r="G604" t="s">
+        <v>126</v>
+      </c>
+      <c r="H604" t="s">
+        <v>36</v>
+      </c>
+      <c r="I604" t="s">
+        <v>33</v>
+      </c>
+      <c r="J604" t="str">
+        <f t="shared" si="0"/>
+        <v>Outcomes of Australian rural clinical schools: a decade of success building the rural medical workforce through the education and training continuum</v>
+      </c>
+      <c r="K604" t="str">
+        <f t="shared" si="1"/>
+        <v>Greenhill, J. A.; Walker, J.; Playford, D.</v>
+      </c>
+      <c r="L604">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="M604">
+        <f t="shared" si="3"/>
+        <v>6.625</v>
+      </c>
+      <c r="N604" t="s">
+        <v>34</v>
+      </c>
+      <c r="O604" t="s">
+        <v>3836</v>
+      </c>
+      <c r="P604" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q604" t="s">
+        <v>33</v>
+      </c>
+      <c r="R604" t="s">
+        <v>33</v>
+      </c>
+      <c r="S604" t="s">
+        <v>33</v>
+      </c>
+      <c r="T604" t="s">
+        <v>33</v>
+      </c>
+      <c r="U604" t="s">
+        <v>33</v>
+      </c>
+      <c r="V604" t="s">
+        <v>33</v>
+      </c>
+      <c r="W604" t="s">
+        <v>33</v>
+      </c>
+      <c r="X604" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y604" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z604" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA604" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB604">
+        <v>0</v>
+      </c>
+      <c r="AC604" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="605" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>3821</v>
+      </c>
+      <c r="B605" t="s">
+        <v>3822</v>
+      </c>
+      <c r="C605" t="s">
+        <v>33</v>
+      </c>
+      <c r="D605">
+        <v>2006</v>
+      </c>
+      <c r="E605">
+        <v>116</v>
+      </c>
+      <c r="F605" t="s">
+        <v>3823</v>
+      </c>
+      <c r="G605" t="s">
+        <v>126</v>
+      </c>
+      <c r="H605" t="s">
+        <v>36</v>
+      </c>
+      <c r="I605" t="s">
+        <v>33</v>
+      </c>
+      <c r="J605" t="str">
+        <f t="shared" si="0"/>
+        <v>Pathogens, nutritional deficiency, and climate influences on a declining moose population</v>
+      </c>
+      <c r="K605" t="str">
+        <f t="shared" si="1"/>
+        <v>Murray, Dennis L.; Cox, Eric W.; Ballard, Warren B.; Whitlaw, Heather A.; Lenarz, Mark S.; Custer, Thomas W.; Barnett, Terri; Fuller, Todd K.</v>
+      </c>
+      <c r="L605">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="M605">
+        <f t="shared" si="3"/>
+        <v>6.8235294117647056</v>
+      </c>
+      <c r="N605" t="s">
+        <v>34</v>
+      </c>
+      <c r="O605" t="s">
+        <v>3834</v>
+      </c>
+      <c r="P605" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q605" t="s">
+        <v>33</v>
+      </c>
+      <c r="R605" t="s">
+        <v>33</v>
+      </c>
+      <c r="S605" t="s">
+        <v>33</v>
+      </c>
+      <c r="T605" t="s">
+        <v>33</v>
+      </c>
+      <c r="U605" t="s">
+        <v>33</v>
+      </c>
+      <c r="V605" t="s">
+        <v>33</v>
+      </c>
+      <c r="W605" t="s">
+        <v>33</v>
+      </c>
+      <c r="X605" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y605" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z605" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA605" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB605">
+        <v>0</v>
+      </c>
+      <c r="AC605" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="606" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>3824</v>
+      </c>
+      <c r="B606" t="s">
+        <v>3825</v>
+      </c>
+      <c r="C606" t="s">
+        <v>33</v>
+      </c>
+      <c r="D606">
+        <v>2021</v>
+      </c>
+      <c r="E606">
+        <v>39</v>
+      </c>
+      <c r="F606" t="s">
+        <v>3826</v>
+      </c>
+      <c r="G606" t="s">
+        <v>126</v>
+      </c>
+      <c r="H606" t="s">
+        <v>36</v>
+      </c>
+      <c r="I606" t="s">
+        <v>33</v>
+      </c>
+      <c r="J606" t="str">
+        <f t="shared" si="0"/>
+        <v>Climate anxiety in children and young people and their beliefs about government responses to climate change: a global survey</v>
+      </c>
+      <c r="K606" t="str">
+        <f t="shared" si="1"/>
+        <v>Hickman, Caroline; Marks, Elizabeth; Pihkala, Panu; Clayton, Susan; Lewandowski, R. Eric; Mayall, Elouise E.; Wray, Britt; Mellor, Catriona; van Susteren, Lise</v>
+      </c>
+      <c r="L606">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="M606">
+        <f t="shared" si="3"/>
+        <v>19.5</v>
+      </c>
+      <c r="N606" t="s">
+        <v>34</v>
+      </c>
+      <c r="O606" t="s">
+        <v>3835</v>
+      </c>
+      <c r="P606" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q606" t="s">
+        <v>33</v>
+      </c>
+      <c r="R606" t="s">
+        <v>33</v>
+      </c>
+      <c r="S606" t="s">
+        <v>33</v>
+      </c>
+      <c r="T606" t="s">
+        <v>33</v>
+      </c>
+      <c r="U606" t="s">
+        <v>33</v>
+      </c>
+      <c r="V606" t="s">
+        <v>33</v>
+      </c>
+      <c r="W606" t="s">
+        <v>33</v>
+      </c>
+      <c r="X606" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y606" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z606" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA606" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB606">
+        <v>0</v>
+      </c>
+      <c r="AC606" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="607" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>3827</v>
+      </c>
+      <c r="B607" t="s">
+        <v>3828</v>
+      </c>
+      <c r="C607" t="s">
+        <v>33</v>
+      </c>
+      <c r="D607">
+        <v>2021</v>
+      </c>
+      <c r="E607">
+        <v>24</v>
+      </c>
+      <c r="F607" t="s">
+        <v>3829</v>
+      </c>
+      <c r="G607" t="s">
+        <v>126</v>
+      </c>
+      <c r="H607" t="s">
+        <v>36</v>
+      </c>
+      <c r="I607" t="s">
+        <v>33</v>
+      </c>
+      <c r="J607" t="str">
+        <f t="shared" si="0"/>
+        <v>Reducing the health effects of hot weather and heat extremes: from personal cooling strategies to green cities</v>
+      </c>
+      <c r="K607" t="str">
+        <f t="shared" si="1"/>
+        <v>Jay, Ollie; Capon, Anthony; Berry, Peter; Broderick, Carolyn; de Dear, Richard; Havenith, George; Honda, Yasushi; Kovats, R. Sari; Ma, Wei; Malik, Arunima; Morris, Nathan B.; Nybo, Lars; Seneviratne, Sonia I.; Vanos, Jennifer; Ebi, Kristie L.</v>
+      </c>
+      <c r="L607">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M607">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N607" t="s">
+        <v>3837</v>
+      </c>
+      <c r="O607" t="s">
+        <v>3838</v>
+      </c>
+      <c r="P607" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q607" t="s">
+        <v>78</v>
+      </c>
+      <c r="R607" t="s">
+        <v>104</v>
+      </c>
+      <c r="S607" t="s">
+        <v>1992</v>
+      </c>
+      <c r="T607" t="s">
+        <v>348</v>
+      </c>
+      <c r="U607" t="s">
+        <v>79</v>
+      </c>
+      <c r="V607" t="s">
+        <v>81</v>
+      </c>
+      <c r="W607" t="s">
+        <v>79</v>
+      </c>
+      <c r="X607" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y607" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z607" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA607" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB607">
+        <v>0</v>
+      </c>
+      <c r="AC607" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="608" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>3830</v>
+      </c>
+      <c r="B608" t="s">
+        <v>3831</v>
+      </c>
+      <c r="C608" t="s">
+        <v>33</v>
+      </c>
+      <c r="D608">
+        <v>2021</v>
+      </c>
+      <c r="E608">
+        <v>28</v>
+      </c>
+      <c r="F608" t="s">
+        <v>3832</v>
+      </c>
+      <c r="G608" t="s">
+        <v>126</v>
+      </c>
+      <c r="H608" t="s">
+        <v>36</v>
+      </c>
+      <c r="I608" t="s">
+        <v>33</v>
+      </c>
+      <c r="J608" t="str">
+        <f t="shared" si="0"/>
+        <v>Climate change and child health: a scoping review and an expanded conceptual framework</v>
+      </c>
+      <c r="K608" t="str">
+        <f t="shared" si="1"/>
+        <v>Hellden, Daniel; Andersson, Camilla; Nilsson, Maria; Ebi, Kristie L.; Friberg, Peter; Alfven, Tobias</v>
+      </c>
+      <c r="L608">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="M608">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="N608" t="s">
+        <v>34</v>
+      </c>
+      <c r="O608" t="s">
+        <v>3835</v>
+      </c>
+      <c r="P608" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q608" t="s">
+        <v>33</v>
+      </c>
+      <c r="R608" t="s">
+        <v>33</v>
+      </c>
+      <c r="S608" t="s">
+        <v>33</v>
+      </c>
+      <c r="T608" t="s">
+        <v>33</v>
+      </c>
+      <c r="U608" t="s">
+        <v>33</v>
+      </c>
+      <c r="V608" t="s">
+        <v>33</v>
+      </c>
+      <c r="W608" t="s">
+        <v>33</v>
+      </c>
+      <c r="X608" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y608" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z608" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA608" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB608">
+        <v>0</v>
+      </c>
+      <c r="AC608" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -67054,7 +67889,7 @@
   <dimension ref="A1:U316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>